<commit_message>
VICI chip (within VIC20Emulator) now working... with all modes and incusing the inverse!.
</commit_message>
<xml_diff>
--- a/docs/C64Data/Characters.xlsx
+++ b/docs/C64Data/Characters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\C64Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0FED68-929C-4527-A6C1-269EB816D95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0378C9A9-57AE-446C-9CFC-685FD8ECCDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{8BB24F7E-EEEF-4DC4-B445-87969509D3BC}"/>
   </bookViews>
@@ -72,14 +72,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -101,9 +94,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -141,7 +134,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -247,7 +240,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,7 +382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -399,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEE827-51B2-4DED-9A97-394114155FC2}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -408,7 +401,7 @@
     <col min="1" max="8" width="2.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>128</v>
       </c>
@@ -442,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -451,7 +444,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -461,7 +454,7 @@
       </c>
       <c r="I2">
         <f>A2*$A$1+B2*$B$1+C2*$C$1+D2*$D$1+E2*$E$1+F2*$F$1+G2*$G$1+H2*$H$1</f>
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -603,12 +596,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:H8">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:H9">
+  <conditionalFormatting sqref="A2:H9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Now C16/116 starts but it still doesn't work. Still pending Cplus4 (ACIA chip is not still configured). Minimum mistakes in VIC20 solved (when drawing borders).
</commit_message>
<xml_diff>
--- a/docs/C64Data/Characters.xlsx
+++ b/docs/C64Data/Characters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\C64Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0378C9A9-57AE-446C-9CFC-685FD8ECCDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B58F34-882E-4E1C-BCC3-69F713753A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{8BB24F7E-EEEF-4DC4-B445-87969509D3BC}"/>
   </bookViews>
@@ -393,7 +393,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -444,7 +444,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -454,7 +454,7 @@
       </c>
       <c r="I2">
         <f>A2*$A$1+B2*$B$1+C2*$C$1+D2*$D$1+E2*$E$1+F2*$F$1+G2*$G$1+H2*$H$1</f>
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -578,18 +578,90 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Improving startup C264. Deepon mistake addressed when configured for specific chips.
</commit_message>
<xml_diff>
--- a/docs/C64Data/Characters.xlsx
+++ b/docs/C64Data/Characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\C64Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B58F34-882E-4E1C-BCC3-69F713753A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37674012-2222-44B8-86E5-21CA53E7725B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{8BB24F7E-EEEF-4DC4-B445-87969509D3BC}"/>
   </bookViews>
@@ -72,7 +72,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -390,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEE827-51B2-4DED-9A97-394114155FC2}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -651,10 +658,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -664,11 +671,46 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10" si="1">A10*$A$1+B10*$B$1+C10*$C$1+D10*$D$1+E10*$E$1+F10*$F$1+G10*$G$1+H10*$H$1</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:H9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:H10">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Now, when the interrupts are requested about whether it their time to be executed, they can returns different states (unsigned int). Three are by default: NO, WAIT, RUN. These different states can be treated by the CPU. The CPU admit a list of pending interrupts. By default, onky one is admited. The interrupts can be desactivate/activated using the command in the console INTSET. The format of the interrupts now sow also whether they are active. A special tester program for Z80 has been created. To test whether all instructions works or not. Needed before progressing with the emulator. After executing this tester many mistakes have been found in many instructions. Not finished.
</commit_message>
<xml_diff>
--- a/docs/C64Data/Characters.xlsx
+++ b/docs/C64Data/Characters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\C64Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37674012-2222-44B8-86E5-21CA53E7725B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D6459B-6BBC-495B-B20C-DD179DD57A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{8BB24F7E-EEEF-4DC4-B445-87969509D3BC}"/>
   </bookViews>
@@ -33,6 +33,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,13 +70,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -397,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEE827-51B2-4DED-9A97-394114155FC2}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -410,58 +429,54 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="B1">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="C1">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D1">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <f>A2*$A$1+B2*$B$1+C2*$C$1+D2*$D$1+E2*$E$1+F2*$F$1+G2*$G$1+H2*$H$1</f>
-        <v>60</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -469,29 +484,29 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I9" si="0">A3*$A$1+B3*$B$1+C3*$C$1+D3*$D$1+E3*$E$1+F3*$F$1+G3*$G$1+H3*$H$1</f>
-        <v>102</v>
+        <f>A3*$A$2+B3*$B$2+C3*$C$2+D3*$D$2+E3*$E$2+F3*$F$2+G3*$G$2+H3*$H$2</f>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -508,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -520,8 +535,8 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>110</v>
+        <f t="shared" ref="I4:I10" si="0">A4*$A$2+B4*$B$2+C4*$C$2+D4*$D$2+E4*$E$2+F4*$F$2+G4*$G$2+H4*$H$2</f>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -568,20 +583,20 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -604,14 +619,14 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -619,29 +634,29 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -652,10 +667,10 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -671,7 +686,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -688,10 +703,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -700,17 +715,147 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10" si="1">A10*$A$1+B10*$B$1+C10*$C$1+D10*$D$1+E10*$E$1+F10*$F$1+G10*$G$1+H10*$H$1</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11" si="1">A11*$A$2+B11*$B$2+C11*$C$2+D11*$D$2+E11*$E$2+F11*$F$2+G11*$G$2+H11*$H$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12" si="2">A12*$A$2+B12*$B$2+C12*$C$2+D12*$D$2+E12*$E$2+F12*$F$2+G12*$G$2+H12*$H$2</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13" si="3">A13*$A$2+B13*$B$2+C13*$C$2+D13*$D$2+E13*$E$2+F13*$F$2+G13*$G$2+H13*$H$2</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14" si="4">A14*$A$2+B14*$B$2+C14*$C$2+D14*$D$2+E14*$E$2+F14*$F$2+G14*$G$2+H14*$H$2</f>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:H9">
+  <conditionalFormatting sqref="A3:H11">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:H12">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:H13">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:H10">
+  <conditionalFormatting sqref="A14:H14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
HERO know works. The way the sprites were drawn was not right. It could happen that a sprite with low priority (higger number) was draw on top of someone with high priority. The way the background and the foreground were prioritized was not right at all. Addtionally the method fromUnsignedInt to create Addresses was not taking into account a fize length in bytes. When the int was in page 0 the address created had 1 byte and 2 were needed. The formatters and the help have been modified to provide more explanation.
</commit_message>
<xml_diff>
--- a/docs/C64Data/Characters.xlsx
+++ b/docs/C64Data/Characters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\C64Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDA7C9C-FB97-486B-B22B-940A7EBB4556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AF57FE-3354-4C72-9C94-BA6A933A936F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{8BB24F7E-EEEF-4DC4-B445-87969509D3BC}"/>
   </bookViews>
@@ -37,9 +37,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,44 +91,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -446,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEE827-51B2-4DED-9A97-394114155FC2}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -457,7 +437,7 @@
     <col min="1" max="8" width="2.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>7</v>
       </c>
@@ -483,33 +463,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2">
+    <row r="2" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="4">
         <v>128</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>64</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>32</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>16</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>8</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>2</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -538,8 +518,12 @@
         <f>A3*$A$2+B3*$B$2+C3*$C$2+D3*$D$2+E3*$E$2+F3*$F$2+G3*$G$2+H3*$H$2</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J3" s="2" t="str">
+        <f>DEC2HEX(I3)</f>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>0</v>
       </c>
@@ -568,8 +552,12 @@
         <f t="shared" ref="I4:I10" si="0">A4*$A$2+B4*$B$2+C4*$C$2+D4*$D$2+E4*$E$2+F4*$F$2+G4*$G$2+H4*$H$2</f>
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J10" si="1">DEC2HEX(I4)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
@@ -598,8 +586,12 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>6E</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0</v>
       </c>
@@ -628,8 +620,12 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>6E</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0</v>
       </c>
@@ -658,8 +654,12 @@
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>0</v>
       </c>
@@ -688,8 +688,12 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>0</v>
       </c>
@@ -718,8 +722,12 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -748,8 +756,12 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11">
         <v>0</v>
       </c>
@@ -775,11 +787,11 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11" si="1">A11*$A$2+B11*$B$2+C11*$C$2+D11*$D$2+E11*$E$2+F11*$F$2+G11*$G$2+H11*$H$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="I11" si="2">A11*$A$2+B11*$B$2+C11*$C$2+D11*$D$2+E11*$E$2+F11*$F$2+G11*$G$2+H11*$H$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>0</v>
       </c>
@@ -805,11 +817,15 @@
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" ref="I12" si="2">A12*$A$2+B12*$B$2+C12*$C$2+D12*$D$2+E12*$E$2+F12*$F$2+G12*$G$2+H12*$H$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="I12" si="3">A12*$A$2+B12*$B$2+C12*$C$2+D12*$D$2+E12*$E$2+F12*$F$2+G12*$G$2+H12*$H$2</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <f>DEC2HEX(I12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>0</v>
       </c>
@@ -835,11 +851,15 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13" si="3">A13*$A$2+B13*$B$2+C13*$C$2+D13*$D$2+E13*$E$2+F13*$F$2+G13*$G$2+H13*$H$2</f>
+        <f t="shared" ref="I13" si="4">A13*$A$2+B13*$B$2+C13*$C$2+D13*$D$2+E13*$E$2+F13*$F$2+G13*$G$2+H13*$H$2</f>
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13" t="str">
+        <f t="shared" ref="J13:J19" si="5">DEC2HEX(I13)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0</v>
       </c>
@@ -865,11 +885,15 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I15" si="4">A14*$A$2+B14*$B$2+C14*$C$2+D14*$D$2+E14*$E$2+F14*$F$2+G14*$G$2+H14*$H$2</f>
+        <f t="shared" ref="I14:I15" si="6">A14*$A$2+B14*$B$2+C14*$C$2+D14*$D$2+E14*$E$2+F14*$F$2+G14*$G$2+H14*$H$2</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J14" t="str">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>0</v>
       </c>
@@ -895,11 +919,15 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J15" t="str">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>0</v>
       </c>
@@ -925,11 +953,15 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16:I20" si="5">A16*$A$2+B16*$B$2+C16*$C$2+D16*$D$2+E16*$E$2+F16*$F$2+G16*$G$2+H16*$H$2</f>
+        <f t="shared" ref="I16:I24" si="7">A16*$A$2+B16*$B$2+C16*$C$2+D16*$D$2+E16*$E$2+F16*$F$2+G16*$G$2+H16*$H$2</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J16" t="str">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>0</v>
       </c>
@@ -955,127 +987,421 @@
         <v>0</v>
       </c>
       <c r="I17">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+      <c r="J17" t="str">
         <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>66</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="3">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="2" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="7"/>
+        <v>47</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f>DEC2HEX(I21)</f>
+        <v>2F</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>247</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" ref="J22:J28" si="8">DEC2HEX(I22)</f>
+        <v>F7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>170</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="8"/>
+        <v>AA</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25:I29" si="9">A25*$A$2+B25*$B$2+C25*$C$2+D25*$D$2+E25*$E$2+F25*$F$2+G25*$G$2+H25*$H$2</f>
+        <v>177</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="8"/>
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="9"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="5"/>
+      <c r="J26" t="str">
+        <f t="shared" si="8"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="3">
-        <v>0</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="5"/>
+      <c r="J27" t="str">
+        <f t="shared" si="8"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A28" s="3">
+        <v>0</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:H15">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16:H16">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:H17">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:H18">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:H19">
+  <conditionalFormatting sqref="A3:H20">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H20">
+  <conditionalFormatting sqref="A21:H29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
T64 file format understood. Some changes in the way the commands are managed. Improvements in the documentation.
</commit_message>
<xml_diff>
--- a/docs/C64Data/Characters.xlsx
+++ b/docs/C64Data/Characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\C64Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AF57FE-3354-4C72-9C94-BA6A933A936F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4385E794-C7F5-4196-A347-08A1F1D0C3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{8BB24F7E-EEEF-4DC4-B445-87969509D3BC}"/>
   </bookViews>
@@ -101,14 +101,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -428,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEE827-51B2-4DED-9A97-394114155FC2}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -741,10 +734,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -754,11 +747,11 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>C</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
@@ -1101,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -1120,45 +1113,45 @@
       </c>
       <c r="I21" s="2">
         <f t="shared" si="7"/>
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="J21" s="2" t="str">
         <f>DEC2HEX(I21)</f>
-        <v>2F</v>
+        <v>F</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <f t="shared" si="7"/>
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" ref="J22:J28" si="8">DEC2HEX(I22)</f>
-        <v>F7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1166,19 +1159,19 @@
         <v>0</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1188,59 +1181,59 @@
       </c>
       <c r="I23">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <f t="shared" si="7"/>
-        <v>170</v>
+        <v>5</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="8"/>
-        <v>AA</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1252,20 +1245,20 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <f t="shared" ref="I25:I29" si="9">A25*$A$2+B25*$B$2+C25*$C$2+D25*$D$2+E25*$E$2+F25*$F$2+G25*$G$2+H25*$H$2</f>
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="8"/>
-        <v>B1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1274,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1290,11 +1283,11 @@
       </c>
       <c r="I26">
         <f t="shared" si="9"/>
-        <v>68</v>
+        <v>212</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="8"/>
-        <v>44</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1302,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1314,21 +1307,21 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <f t="shared" si="9"/>
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1336,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -1358,11 +1351,11 @@
       </c>
       <c r="I28" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="J28" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
@@ -1396,12 +1389,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:H20">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21:H29">
+  <conditionalFormatting sqref="A3:H29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>